<commit_message>
fixing parametric and adding tpr, fpr result for every delta
</commit_message>
<xml_diff>
--- a/result/TPR.xlsx
+++ b/result/TPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Research\StatiscalLearning\SI_WDGRL\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26BEDA3-8DA0-4CF3-98B4-2031FBC5F51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97889EC4-E059-4E4E-BEAE-3DB93107D7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,28 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Delta\Method</t>
   </si>
   <si>
-    <t>OC</t>
+    <t>FPR</t>
   </si>
   <si>
-    <t>Parametric</t>
+    <t>OC_TPR</t>
+  </si>
+  <si>
+    <t>Parametric_TPR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,8 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,50 +367,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="C2" s="1">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5.3846153846153801E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>0.241666666666666</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5.83333333333333E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="C4" s="1">
+        <v>0.504132231404958</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.1666666666666602E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.85123966942148699</v>
+      </c>
+      <c r="D5">
+        <v>6.6666666666666596E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding oc_tpr and comparing results
</commit_message>
<xml_diff>
--- a/result/TPR.xlsx
+++ b/result/TPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Research\StatiscalLearning\SI_WDGRL\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97889EC4-E059-4E4E-BEAE-3DB93107D7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60AED4B-93DF-43BA-8EED-176CAC182030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -370,13 +370,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -397,6 +399,9 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>9.0909090909090898E-2</v>
+      </c>
       <c r="C2" s="1">
         <v>9.0909090909090898E-2</v>
       </c>
@@ -408,6 +413,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>0.19008264462809901</v>
+      </c>
       <c r="C3">
         <v>0.241666666666666</v>
       </c>
@@ -419,6 +427,9 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>0.27272727272727199</v>
+      </c>
       <c r="C4" s="1">
         <v>0.504132231404958</v>
       </c>
@@ -429,6 +440,9 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.330578512396694</v>
       </c>
       <c r="C5">
         <v>0.85123966942148699</v>

</xml_diff>

<commit_message>
fixing oc_wdgrl_si and result
</commit_message>
<xml_diff>
--- a/result/TPR.xlsx
+++ b/result/TPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Research\StatiscalLearning\SI_WDGRL\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60AED4B-93DF-43BA-8EED-176CAC182030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113DE8DE-AAB7-4666-ADFB-092B799A3183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,7 +400,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9.0909090909090898E-2</v>
+        <v>6.6115702479338803E-2</v>
       </c>
       <c r="C2" s="1">
         <v>9.0909090909090898E-2</v>
@@ -414,7 +414,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.19008264462809901</v>
+        <v>0.14049586776859499</v>
       </c>
       <c r="C3">
         <v>0.241666666666666</v>
@@ -428,7 +428,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.27272727272727199</v>
+        <v>0.23140495867768501</v>
       </c>
       <c r="C4" s="1">
         <v>0.504132231404958</v>
@@ -442,7 +442,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.330578512396694</v>
+        <v>0.32231404958677601</v>
       </c>
       <c r="C5">
         <v>0.85123966942148699</v>

</xml_diff>